<commit_message>
Set coal and gas to bid at expected capacity factors
</commit_message>
<xml_diff>
--- a/InputData/elec/BDSBaPCF/Boolean Do Suppliers Bid at Peak Capacity Factors.xlsx
+++ b/InputData/elec/BDSBaPCF/Boolean Do Suppliers Bid at Peak Capacity Factors.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\elec\BDSBaPCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-eu\InputData\elec\BDSBaPCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEA2AB1-3804-4241-90B3-B98E7C7ABA50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39555" yWindow="4515" windowWidth="13635" windowHeight="16125" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39555" yWindow="4515" windowWidth="13635" windowHeight="16125"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BDSBaPCF" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>BDSBaPCF Boolean Do Suppliers Bid at Peak Capacity Factors</t>
   </si>
@@ -143,12 +142,18 @@
   </si>
   <si>
     <t>Some plant types are thus set to 1 so that they have the flexibility to bid at higher capacity factors.</t>
+  </si>
+  <si>
+    <t>However, we do not allow coal and gas to bid at their peak capacity factor to avoid overdispatch</t>
+  </si>
+  <si>
+    <t>of either type based on dispatch costs.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -285,23 +290,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -337,23 +325,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -529,11 +500,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -591,53 +562,63 @@
         <v>37</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>25</v>
       </c>
     </row>
@@ -647,14 +628,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -673,7 +654,7 @@
         <v>28</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -681,7 +662,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -761,7 +742,7 @@
         <v>27</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Revert BDSBaPCF to original settings
</commit_message>
<xml_diff>
--- a/InputData/elec/BDSBaPCF/Boolean Do Suppliers Bid at Peak Capacity Factors.xlsx
+++ b/InputData/elec/BDSBaPCF/Boolean Do Suppliers Bid at Peak Capacity Factors.xlsx
@@ -1,29 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-eu\InputData\elec\BDSBaPCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-eu\InputData\elec\BDSBaPCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE38CCD-FDC2-4920-A290-1BCD3C8D2D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39555" yWindow="4515" windowWidth="13635" windowHeight="16125"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BDSBaPCF" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -153,7 +146,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -290,6 +283,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -325,6 +335,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -500,21 +527,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -522,102 +549,102 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -628,7 +655,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -638,34 +665,34 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.59765625" customWidth="1"/>
-    <col min="2" max="2" width="23.1328125" customWidth="1"/>
+    <col min="1" max="1" width="23.6328125" customWidth="1"/>
+    <col min="2" max="2" width="23.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -673,7 +700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -681,7 +708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -689,7 +716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -697,7 +724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -705,7 +732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -713,7 +740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -721,7 +748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -729,7 +756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -737,15 +764,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>27</v>
       </c>
       <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -753,7 +780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -761,7 +788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -769,7 +796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Set biomass and MSW plants to 0 in BDSBaPCF
</commit_message>
<xml_diff>
--- a/InputData/elec/BDSBaPCF/Boolean Do Suppliers Bid at Peak Capacity Factors.xlsx
+++ b/InputData/elec/BDSBaPCF/Boolean Do Suppliers Bid at Peak Capacity Factors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-eu\InputData\elec\BDSBaPCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE38CCD-FDC2-4920-A290-1BCD3C8D2D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC46C6C8-0B51-43EB-AA20-EC1FDC4AFB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,18 @@
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BDSBaPCF" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -662,7 +673,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,7 +748,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -801,7 +812,7 @@
         <v>33</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>